<commit_message>
removed tmp ms files
</commit_message>
<xml_diff>
--- a/pgparallel/stats1.xlsx
+++ b/pgparallel/stats1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="1040" windowWidth="33500" windowHeight="27240" tabRatio="500"/>
+    <workbookView xWindow="6420" yWindow="1040" windowWidth="41260" windowHeight="27420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="14">
   <si>
     <t>Table</t>
   </si>
@@ -653,464 +653,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Sample1</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>temps par worker</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$6:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$6:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>406.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>138.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>111.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>105.3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-2142507040"/>
-        <c:axId val="-2142499200"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="-2142507040"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Workers</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-2142499200"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-2142499200"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>temps (s)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-2142507040"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Sample0</a:t>
             </a:r>
           </a:p>
@@ -1534,7 +1076,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -1641,8 +1183,8 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:r>
-                      <a:rPr lang="hr-HR"/>
-                      <a:t>x3.7</a:t>
+                      <a:rPr lang="en-US"/>
+                      <a:t>x3</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -1801,7 +1343,7 @@
                   <c:v>81.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>21.0</c:v>
@@ -1930,6 +1472,7 @@
         <c:crossAx val="-2142386272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="20.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2008,7 +1551,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -2115,8 +1658,8 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:r>
-                      <a:rPr lang="is-IS"/>
-                      <a:t>x2</a:t>
+                      <a:rPr lang="hr-HR"/>
+                      <a:t>x2.1</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -2275,7 +1818,7 @@
                   <c:v>408.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>205.0</c:v>
+                  <c:v>190.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>103.0</c:v>
@@ -2405,6 +1948,7 @@
         <c:crossAx val="-2137830464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="100.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2483,7 +2027,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -2636,7 +2180,7 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="nb-NO"/>
-                      <a:t>x1.1</a:t>
+                      <a:t>x1.8</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -2794,7 +2338,7 @@
                   <c:v>2010.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1820.0</c:v>
+                  <c:v>1150.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>720.0</c:v>
@@ -3002,7 +2546,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -3083,7 +2627,12 @@
           <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>sample0</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$A$85:$B$85</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -3098,6 +2647,115 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>x1</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="nb-NO"/>
+                      <a:t>x1.7</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="hr-HR"/>
+                      <a:t>x3.9</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="hr-HR"/>
+                      <a:t>x3.6</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="General" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -3185,7 +2843,7 @@
                   <c:v>15122.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10831.0</c:v>
+                  <c:v>8900.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3883.0</c:v>
@@ -3315,6 +2973,7 @@
         <c:crossAx val="-2075810432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="4000.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3356,6 +3015,402 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>sample1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$6:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>406.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>111.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2043210032"/>
+        <c:axId val="-2115665728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2043210032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>workers</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2115665728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2115665728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>temps (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2043210032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="100.0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4706,7 +4761,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4763,7 +4818,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -4815,9 +4870,11 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -4830,16 +4887,18 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -4865,9 +4924,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4880,7 +4936,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -4923,22 +4979,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5043,8 +5100,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5176,19 +5233,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -6779,7 +6837,7 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6836,7 +6894,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -6888,11 +6946,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -6905,18 +6961,16 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -6942,6 +6996,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6954,7 +7011,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -6997,23 +7054,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -7118,8 +7174,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -7251,20 +7307,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -7331,36 +7386,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>275597</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>2074</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>700659</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>49764</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>267824</xdr:colOff>
       <xdr:row>15</xdr:row>
@@ -7385,7 +7410,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7415,7 +7440,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7447,7 +7472,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7479,7 +7504,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7504,6 +7529,36 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>711891</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>27993</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>307565</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>75683</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -7785,8 +7840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="147" zoomScaleNormal="147" zoomScalePageLayoutView="147" workbookViewId="0">
-      <selection activeCell="K69" sqref="K69"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="147" zoomScaleNormal="147" zoomScalePageLayoutView="147" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7897,7 +7952,7 @@
         <v>138.5</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" ref="E7:E9" si="1">D$6/D7</f>
+        <f t="shared" ref="E7:E8" si="1">D$6/D7</f>
         <v>2.9350180505415162</v>
       </c>
     </row>
@@ -7920,22 +7975,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>105.3</v>
-      </c>
-      <c r="E9" s="3">
-        <f t="shared" si="1"/>
-        <v>3.8603988603988606</v>
-      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -8187,11 +8227,11 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" ref="D52:D69" si="3">C$51/C52</f>
-        <v>3.6818181818181817</v>
+        <f t="shared" ref="D52:D54" si="3">C$51/C52</f>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -8250,11 +8290,11 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="D57" s="1">
         <f t="shared" ref="D57:D59" si="4">C$56/C57</f>
-        <v>1.9902439024390244</v>
+        <v>2.1473684210526316</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -8313,11 +8353,11 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <v>1820</v>
+        <v>1150</v>
       </c>
       <c r="D62" s="1">
         <f t="shared" ref="D62:D64" si="5">C$61/C62</f>
-        <v>1.1043956043956045</v>
+        <v>1.7478260869565216</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -8376,11 +8416,11 @@
         <v>9</v>
       </c>
       <c r="C67">
-        <v>10831</v>
+        <v>8900</v>
       </c>
       <c r="D67" s="1">
         <f t="shared" ref="D67:D69" si="6">C$66/C67</f>
-        <v>1.3961776382605484</v>
+        <v>1.6991011235955056</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>